<commit_message>
Updated weather and capacity data
</commit_message>
<xml_diff>
--- a/datasets/historic_wind_speed.xlsx
+++ b/datasets/historic_wind_speed.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasjohannesen/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sambaad.stud.ntnu.no\anjohann\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23C39FD5-6473-8947-94BC-D4063C27B9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{793E11E6-FD80-4273-B56F-234D8757ECF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{799EA429-A02C-486C-A602-0719BD9BF84B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{799EA429-A02C-486C-A602-0719BD9BF84B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!#REF!</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -410,16 +404,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73725F40-D26E-4E9A-8107-C74A02EA9D5D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B205"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206:C217"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>37257</v>
       </c>
@@ -435,7 +432,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>37288</v>
       </c>
@@ -443,7 +440,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>37316</v>
       </c>
@@ -451,7 +448,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>37347</v>
       </c>
@@ -459,7 +456,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>37377</v>
       </c>
@@ -467,7 +464,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>37408</v>
       </c>
@@ -475,7 +472,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>37438</v>
       </c>
@@ -483,7 +480,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>37469</v>
       </c>
@@ -491,7 +488,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>37500</v>
       </c>
@@ -499,7 +496,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>37530</v>
       </c>
@@ -507,7 +504,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>37561</v>
       </c>
@@ -515,7 +512,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>37591</v>
       </c>
@@ -523,7 +520,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>37622</v>
       </c>
@@ -531,7 +528,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>37653</v>
       </c>
@@ -539,7 +536,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>37681</v>
       </c>
@@ -547,7 +544,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>37712</v>
       </c>
@@ -555,7 +552,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37742</v>
       </c>
@@ -563,7 +560,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>37773</v>
       </c>
@@ -571,7 +568,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>37803</v>
       </c>
@@ -579,7 +576,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>37834</v>
       </c>
@@ -587,7 +584,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>37865</v>
       </c>
@@ -595,7 +592,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>37895</v>
       </c>
@@ -603,7 +600,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>37926</v>
       </c>
@@ -611,7 +608,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>37956</v>
       </c>
@@ -619,7 +616,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>37987</v>
       </c>
@@ -627,7 +624,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38018</v>
       </c>
@@ -635,7 +632,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38047</v>
       </c>
@@ -643,7 +640,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>38078</v>
       </c>
@@ -651,7 +648,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>38108</v>
       </c>
@@ -659,7 +656,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>38139</v>
       </c>
@@ -667,7 +664,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>38169</v>
       </c>
@@ -675,7 +672,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>38200</v>
       </c>
@@ -683,7 +680,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>38231</v>
       </c>
@@ -691,7 +688,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>38261</v>
       </c>
@@ -699,7 +696,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>38292</v>
       </c>
@@ -707,7 +704,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>38322</v>
       </c>
@@ -715,7 +712,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>38353</v>
       </c>
@@ -723,7 +720,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38384</v>
       </c>
@@ -731,7 +728,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38412</v>
       </c>
@@ -739,7 +736,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38443</v>
       </c>
@@ -747,7 +744,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38473</v>
       </c>
@@ -755,7 +752,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>38504</v>
       </c>
@@ -763,7 +760,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>38534</v>
       </c>
@@ -771,7 +768,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>38565</v>
       </c>
@@ -779,7 +776,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>38596</v>
       </c>
@@ -787,7 +784,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38626</v>
       </c>
@@ -795,7 +792,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>38657</v>
       </c>
@@ -803,7 +800,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>38687</v>
       </c>
@@ -811,7 +808,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>38718</v>
       </c>
@@ -819,7 +816,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>38749</v>
       </c>
@@ -827,7 +824,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>38777</v>
       </c>
@@ -835,7 +832,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>38808</v>
       </c>
@@ -843,7 +840,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>38838</v>
       </c>
@@ -851,7 +848,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>38869</v>
       </c>
@@ -859,7 +856,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>38899</v>
       </c>
@@ -867,7 +864,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>38930</v>
       </c>
@@ -875,7 +872,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>38961</v>
       </c>
@@ -883,7 +880,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>38991</v>
       </c>
@@ -891,7 +888,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>39022</v>
       </c>
@@ -899,7 +896,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>39052</v>
       </c>
@@ -907,7 +904,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>39083</v>
       </c>
@@ -915,7 +912,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>39114</v>
       </c>
@@ -923,7 +920,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>39142</v>
       </c>
@@ -931,7 +928,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>39173</v>
       </c>
@@ -939,7 +936,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>39203</v>
       </c>
@@ -947,7 +944,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>39234</v>
       </c>
@@ -955,7 +952,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>39264</v>
       </c>
@@ -963,7 +960,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>39295</v>
       </c>
@@ -971,7 +968,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>39326</v>
       </c>
@@ -979,7 +976,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>39356</v>
       </c>
@@ -987,7 +984,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>39387</v>
       </c>
@@ -995,7 +992,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>39417</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>39448</v>
       </c>
@@ -1011,7 +1008,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>39479</v>
       </c>
@@ -1019,7 +1016,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>39508</v>
       </c>
@@ -1027,7 +1024,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>39539</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>39569</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>39600</v>
       </c>
@@ -1051,7 +1048,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>39630</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>39661</v>
       </c>
@@ -1067,7 +1064,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39692</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>39722</v>
       </c>
@@ -1083,7 +1080,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>39753</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>39783</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>39814</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>39845</v>
       </c>
@@ -1115,7 +1112,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>39873</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>39904</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>39934</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>39965</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>39995</v>
       </c>
@@ -1155,7 +1152,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>40026</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>40057</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>40087</v>
       </c>
@@ -1179,7 +1176,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>40118</v>
       </c>
@@ -1187,7 +1184,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>40148</v>
       </c>
@@ -1195,7 +1192,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>40179</v>
       </c>
@@ -1203,7 +1200,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>40210</v>
       </c>
@@ -1211,7 +1208,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>40238</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>40269</v>
       </c>
@@ -1227,7 +1224,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>40299</v>
       </c>
@@ -1235,7 +1232,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>40330</v>
       </c>
@@ -1243,7 +1240,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>40360</v>
       </c>
@@ -1251,7 +1248,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>40391</v>
       </c>
@@ -1259,7 +1256,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>40422</v>
       </c>
@@ -1267,7 +1264,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>40452</v>
       </c>
@@ -1275,7 +1272,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>40483</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>40513</v>
       </c>
@@ -1291,7 +1288,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>40544</v>
       </c>
@@ -1299,7 +1296,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>40575</v>
       </c>
@@ -1307,7 +1304,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>40603</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>40634</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>40664</v>
       </c>
@@ -1331,7 +1328,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>40695</v>
       </c>
@@ -1339,7 +1336,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>40725</v>
       </c>
@@ -1347,7 +1344,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>40756</v>
       </c>
@@ -1355,7 +1352,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>40787</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>40817</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>40848</v>
       </c>
@@ -1379,7 +1376,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>40878</v>
       </c>
@@ -1387,7 +1384,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>40909</v>
       </c>
@@ -1395,7 +1392,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>40940</v>
       </c>
@@ -1403,7 +1400,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>40969</v>
       </c>
@@ -1411,7 +1408,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>41000</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>41030</v>
       </c>
@@ -1427,7 +1424,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>41061</v>
       </c>
@@ -1435,7 +1432,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>41091</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>41122</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>41153</v>
       </c>
@@ -1459,7 +1456,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>41183</v>
       </c>
@@ -1467,7 +1464,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>41214</v>
       </c>
@@ -1475,7 +1472,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>41244</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>41275</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>41306</v>
       </c>
@@ -1499,7 +1496,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>41334</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>41365</v>
       </c>
@@ -1515,7 +1512,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>41395</v>
       </c>
@@ -1523,7 +1520,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>41426</v>
       </c>
@@ -1531,7 +1528,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>41456</v>
       </c>
@@ -1539,7 +1536,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>41487</v>
       </c>
@@ -1547,7 +1544,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>41518</v>
       </c>
@@ -1555,7 +1552,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>41548</v>
       </c>
@@ -1563,7 +1560,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>41579</v>
       </c>
@@ -1571,7 +1568,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>41609</v>
       </c>
@@ -1579,7 +1576,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>41640</v>
       </c>
@@ -1587,7 +1584,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>41671</v>
       </c>
@@ -1595,7 +1592,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>41699</v>
       </c>
@@ -1603,7 +1600,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>41730</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>41760</v>
       </c>
@@ -1619,7 +1616,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>41791</v>
       </c>
@@ -1627,7 +1624,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>41821</v>
       </c>
@@ -1635,7 +1632,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>41852</v>
       </c>
@@ -1643,7 +1640,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>41883</v>
       </c>
@@ -1651,7 +1648,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>41913</v>
       </c>
@@ -1659,7 +1656,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>41944</v>
       </c>
@@ -1667,7 +1664,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>41974</v>
       </c>
@@ -1675,7 +1672,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>42005</v>
       </c>
@@ -1683,7 +1680,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>42036</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>42064</v>
       </c>
@@ -1699,7 +1696,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>42095</v>
       </c>
@@ -1707,7 +1704,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>42125</v>
       </c>
@@ -1715,7 +1712,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>42156</v>
       </c>
@@ -1723,7 +1720,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>42186</v>
       </c>
@@ -1731,7 +1728,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>42217</v>
       </c>
@@ -1739,7 +1736,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>42248</v>
       </c>
@@ -1747,7 +1744,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>42278</v>
       </c>
@@ -1755,7 +1752,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>42309</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>42339</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>42370</v>
       </c>
@@ -1779,7 +1776,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>42401</v>
       </c>
@@ -1787,7 +1784,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>42430</v>
       </c>
@@ -1795,7 +1792,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>42461</v>
       </c>
@@ -1803,7 +1800,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>42491</v>
       </c>
@@ -1811,7 +1808,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>42522</v>
       </c>
@@ -1819,7 +1816,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>42552</v>
       </c>
@@ -1827,7 +1824,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>42583</v>
       </c>
@@ -1835,7 +1832,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>42614</v>
       </c>
@@ -1843,7 +1840,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>42644</v>
       </c>
@@ -1851,7 +1848,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>42675</v>
       </c>
@@ -1859,7 +1856,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>42705</v>
       </c>
@@ -1867,7 +1864,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>42736</v>
       </c>
@@ -1875,7 +1872,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>42767</v>
       </c>
@@ -1883,7 +1880,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>42795</v>
       </c>
@@ -1891,7 +1888,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>42826</v>
       </c>
@@ -1899,7 +1896,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>42856</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>42887</v>
       </c>
@@ -1915,7 +1912,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>42917</v>
       </c>
@@ -1923,7 +1920,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>42948</v>
       </c>
@@ -1931,7 +1928,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>42979</v>
       </c>
@@ -1939,7 +1936,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43009</v>
       </c>
@@ -1947,7 +1944,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>43040</v>
       </c>
@@ -1955,7 +1952,7 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43070</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>923.90000000000009</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>43101</v>
       </c>
@@ -1971,7 +1968,7 @@
         <v>998.59999999999991</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>43132</v>
       </c>
@@ -1979,7 +1976,7 @@
         <v>899.40000000000009</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43160</v>
       </c>
@@ -1987,7 +1984,7 @@
         <v>893.39999999999986</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43191</v>
       </c>
@@ -1995,7 +1992,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>43221</v>
       </c>
@@ -2003,7 +2000,7 @@
         <v>596.1</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>43252</v>
       </c>
@@ -2011,7 +2008,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43282</v>
       </c>
@@ -2019,7 +2016,7 @@
         <v>568.99999999999989</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43313</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>572.79999999999995</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43344</v>
       </c>
@@ -2035,7 +2032,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43374</v>
       </c>
@@ -2043,7 +2040,7 @@
         <v>684.5</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43405</v>
       </c>
@@ -2051,13 +2048,121 @@
         <v>743.6</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43435</v>
       </c>
       <c r="B205">
         <v>923.90000000000009</v>
       </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B206">
+        <v>998.59999999999991</v>
+      </c>
+      <c r="C206" s="1"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B207">
+        <v>899.40000000000009</v>
+      </c>
+      <c r="C207" s="1"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B208">
+        <v>893.39999999999986</v>
+      </c>
+      <c r="C208" s="1"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B209">
+        <v>656.5</v>
+      </c>
+      <c r="C209" s="1"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B210">
+        <v>596.1</v>
+      </c>
+      <c r="C210" s="1"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B211">
+        <v>580.9</v>
+      </c>
+      <c r="C211" s="1"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B212">
+        <v>568.99999999999989</v>
+      </c>
+      <c r="C212" s="1"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B213">
+        <v>572.79999999999995</v>
+      </c>
+      <c r="C213" s="1"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B214">
+        <v>586.20000000000005</v>
+      </c>
+      <c r="C214" s="1"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B215">
+        <v>684.5</v>
+      </c>
+      <c r="C215" s="1"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B216">
+        <v>743.6</v>
+      </c>
+      <c r="C216" s="1"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B217">
+        <v>923.90000000000009</v>
+      </c>
+      <c r="C217" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>